<commit_message>
--ffiaf XL output labeled with B- and V-
</commit_message>
<xml_diff>
--- a/output/combinedrepos/combinedrepos-bug-fiaf.xlsx
+++ b/output/combinedrepos/combinedrepos-bug-fiaf.xlsx
@@ -756,7 +756,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>php:S905</t>
+          <t>B-php:S905</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -958,7 +958,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>javascript:S2259</t>
+          <t>B-javascript:S2259</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1160,7 +1160,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>php:S836</t>
+          <t>B-php:S836</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1362,7 +1362,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>php:S2201</t>
+          <t>B-php:S2201</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1564,7 +1564,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>php:S1764</t>
+          <t>B-php:S1764</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1766,7 +1766,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>javascript:S2137</t>
+          <t>B-javascript:S2137</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1968,7 +1968,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>javascript:DuplicatePropertyName</t>
+          <t>B-javascript:DuplicatePropertyName</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2170,7 +2170,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>javascript:S3981</t>
+          <t>B-javascript:S3981</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2372,7 +2372,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>javascript:S2583</t>
+          <t>B-javascript:S2583</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2574,7 +2574,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>javascript:S3812</t>
+          <t>B-javascript:S3812</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2776,7 +2776,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>javascript:S905</t>
+          <t>B-javascript:S905</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2978,7 +2978,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>javascript:S3001</t>
+          <t>B-javascript:S3001</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -3180,7 +3180,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>javascript:S3403</t>
+          <t>B-javascript:S3403</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -3382,7 +3382,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>javascript:S2201</t>
+          <t>B-javascript:S2201</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -3584,7 +3584,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>php:S1848</t>
+          <t>B-php:S1848</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -3786,7 +3786,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>php:S1656</t>
+          <t>B-php:S1656</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -3988,7 +3988,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>php:S3923</t>
+          <t>B-php:S3923</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -4190,7 +4190,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Web:BoldAndItalicTagsCheck</t>
+          <t>B-Web:BoldAndItalicTagsCheck</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -4392,7 +4392,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>javascript:S2757</t>
+          <t>B-javascript:S2757</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -4594,7 +4594,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>php:S1763</t>
+          <t>B-php:S1763</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -4796,7 +4796,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>javascript:S2873</t>
+          <t>B-javascript:S2873</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -4998,7 +4998,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>javascript:S1143</t>
+          <t>B-javascript:S1143</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -5200,7 +5200,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>javascript:UnreachableCode</t>
+          <t>B-javascript:UnreachableCode</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -5402,7 +5402,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>javascript:S3785</t>
+          <t>B-javascript:S3785</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -5604,7 +5604,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>php:S1862</t>
+          <t>B-php:S1862</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -5806,7 +5806,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Web:DoctypePresenceCheck</t>
+          <t>B-Web:DoctypePresenceCheck</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -6008,7 +6008,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Web:FieldsetWithoutLegendCheck</t>
+          <t>B-Web:FieldsetWithoutLegendCheck</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -6210,7 +6210,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>php:S2757</t>
+          <t>B-php:S2757</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -6412,7 +6412,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Web:PageWithoutTitleCheck</t>
+          <t>B-Web:PageWithoutTitleCheck</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -6614,7 +6614,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>javascript:S1656</t>
+          <t>B-javascript:S1656</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -6816,7 +6816,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Web:ImgWithoutAltCheck</t>
+          <t>B-Web:ImgWithoutAltCheck</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -7018,7 +7018,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>javascript:S4043</t>
+          <t>B-javascript:S4043</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -7220,7 +7220,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>php:S1145</t>
+          <t>B-php:S1145</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -7422,7 +7422,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Web:UnsupportedTagsInHtml5Check</t>
+          <t>B-Web:UnsupportedTagsInHtml5Check</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -7624,7 +7624,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Web:FrameWithoutTitleCheck</t>
+          <t>B-Web:FrameWithoutTitleCheck</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -7826,7 +7826,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>php:S3699</t>
+          <t>B-php:S3699</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -8028,7 +8028,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>javascript:S2189</t>
+          <t>B-javascript:S2189</t>
         </is>
       </c>
       <c r="B38" t="n">

</xml_diff>